<commit_message>
Add post form with shift type (day/night)
</commit_message>
<xml_diff>
--- a/ガードプール_技術仕様書_スケジュール.xlsx
+++ b/ガードプール_技術仕様書_スケジュール.xlsx
@@ -531,7 +531,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,7 +555,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>作成日: 2026年02月02日</t>
+          <t>作成日: 2026年02月03日</t>
         </is>
       </c>
     </row>
@@ -1172,35 +1172,27 @@
     <row r="45">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>HTTPS</t>
-        </is>
-      </c>
-      <c r="B45" s="4" t="inlineStr">
-        <is>
-          <t>対応</t>
-        </is>
-      </c>
-      <c r="C45" s="4" t="inlineStr">
-        <is>
-          <t>Netlify標準</t>
-        </is>
-      </c>
+          <t>現状（Phase 1）</t>
+        </is>
+      </c>
+      <c r="B45" s="4" t="inlineStr"/>
+      <c r="C45" s="4" t="inlineStr"/>
       <c r="D45" s="4" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="4" t="inlineStr">
         <is>
-          <t>パスワード</t>
+          <t>HTTPS</t>
         </is>
       </c>
       <c r="B46" s="4" t="inlineStr">
         <is>
-          <t>平文保存（暫定）</t>
+          <t>対応</t>
         </is>
       </c>
       <c r="C46" s="4" t="inlineStr">
         <is>
-          <t>将来的にハッシュ化推奨</t>
+          <t>Netlify標準</t>
         </is>
       </c>
       <c r="D46" s="4" t="inlineStr"/>
@@ -1208,20 +1200,214 @@
     <row r="47">
       <c r="A47" s="4" t="inlineStr">
         <is>
+          <t>パスワード</t>
+        </is>
+      </c>
+      <c r="B47" s="4" t="inlineStr">
+        <is>
+          <t>平文保存（暫定）</t>
+        </is>
+      </c>
+      <c r="C47" s="4" t="inlineStr">
+        <is>
+          <t>基本機能優先</t>
+        </is>
+      </c>
+      <c r="D47" s="4" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="4" t="inlineStr">
+        <is>
           <t>アクセス制限</t>
         </is>
       </c>
-      <c r="B47" s="4" t="inlineStr">
+      <c r="B48" s="4" t="inlineStr">
         <is>
           <t>ログイン必須</t>
         </is>
       </c>
-      <c r="C47" s="4" t="inlineStr">
+      <c r="C48" s="4" t="inlineStr">
         <is>
           <t>未ログインは index.html へリダイレクト</t>
         </is>
       </c>
-      <c r="D47" s="4" t="inlineStr"/>
+      <c r="D48" s="4" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="4" t="inlineStr"/>
+      <c r="B49" s="4" t="inlineStr"/>
+      <c r="C49" s="4" t="inlineStr"/>
+      <c r="D49" s="4" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="4" t="inlineStr">
+        <is>
+          <t>アルファテクノロジー依頼項目（Phase 2）</t>
+        </is>
+      </c>
+      <c r="B50" s="4" t="inlineStr"/>
+      <c r="C50" s="4" t="inlineStr"/>
+      <c r="D50" s="4" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="inlineStr">
+        <is>
+          <t>パスワードハッシュ化</t>
+        </is>
+      </c>
+      <c r="B51" s="4" t="inlineStr">
+        <is>
+          <t>bcrypt / Argon2</t>
+        </is>
+      </c>
+      <c r="C51" s="4" t="inlineStr">
+        <is>
+          <t>セキュリティ強化</t>
+        </is>
+      </c>
+      <c r="D51" s="4" t="inlineStr">
+        <is>
+          <t>親会社IT部門に依頼</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="inlineStr">
+        <is>
+          <t>SSL/TLS通信</t>
+        </is>
+      </c>
+      <c r="B52" s="4" t="inlineStr">
+        <is>
+          <t>全通信の暗号化</t>
+        </is>
+      </c>
+      <c r="C52" s="4" t="inlineStr">
+        <is>
+          <t>データ盗聴防止</t>
+        </is>
+      </c>
+      <c r="D52" s="4" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="4" t="inlineStr">
+        <is>
+          <t>アクセスログ</t>
+        </is>
+      </c>
+      <c r="B53" s="4" t="inlineStr">
+        <is>
+          <t>ログイン・操作履歴記録</t>
+        </is>
+      </c>
+      <c r="C53" s="4" t="inlineStr">
+        <is>
+          <t>不正アクセス検知</t>
+        </is>
+      </c>
+      <c r="D53" s="4" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="4" t="inlineStr">
+        <is>
+          <t>データバックアップ</t>
+        </is>
+      </c>
+      <c r="B54" s="4" t="inlineStr">
+        <is>
+          <t>自動バックアップ（日次）</t>
+        </is>
+      </c>
+      <c r="C54" s="4" t="inlineStr">
+        <is>
+          <t>データ保護</t>
+        </is>
+      </c>
+      <c r="D54" s="4" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="4" t="inlineStr">
+        <is>
+          <t>IPアドレス制限</t>
+        </is>
+      </c>
+      <c r="B55" s="4" t="inlineStr">
+        <is>
+          <t>登録企業のみアクセス可能</t>
+        </is>
+      </c>
+      <c r="C55" s="4" t="inlineStr">
+        <is>
+          <t>不正アクセス防止</t>
+        </is>
+      </c>
+      <c r="D55" s="4" t="inlineStr">
+        <is>
+          <t>オプション</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="inlineStr">
+        <is>
+          <t>二段階認証</t>
+        </is>
+      </c>
+      <c r="B56" s="4" t="inlineStr">
+        <is>
+          <t>SMS / メール認証</t>
+        </is>
+      </c>
+      <c r="C56" s="4" t="inlineStr">
+        <is>
+          <t>セキュリティ強化</t>
+        </is>
+      </c>
+      <c r="D56" s="4" t="inlineStr">
+        <is>
+          <t>将来的に検討</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="4" t="inlineStr">
+        <is>
+          <t>監査ログ</t>
+        </is>
+      </c>
+      <c r="B57" s="4" t="inlineStr">
+        <is>
+          <t>操作履歴の長期保存</t>
+        </is>
+      </c>
+      <c r="C57" s="4" t="inlineStr">
+        <is>
+          <t>コンプライアンス対応</t>
+        </is>
+      </c>
+      <c r="D57" s="4" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="4" t="inlineStr">
+        <is>
+          <t>脆弱性診断</t>
+        </is>
+      </c>
+      <c r="B58" s="4" t="inlineStr">
+        <is>
+          <t>定期的なセキュリティ診断</t>
+        </is>
+      </c>
+      <c r="C58" s="4" t="inlineStr">
+        <is>
+          <t>脆弱性の早期発見</t>
+        </is>
+      </c>
+      <c r="D58" s="4" t="inlineStr">
+        <is>
+          <t>年1回実施</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1370,19 +1556,19 @@
       <c r="E9" s="9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="inlineStr">
-        <is>
-          <t>❌ 未完了</t>
+      <c r="A10" s="8" t="inlineStr">
+        <is>
+          <t>✅ 完了</t>
         </is>
       </c>
       <c r="B10" s="9" t="inlineStr">
         <is>
-          <t>投稿機能</t>
+          <t>投稿一覧表示</t>
         </is>
       </c>
       <c r="C10" s="9" t="inlineStr">
         <is>
-          <t>開発中</t>
+          <t>ダミーデータで表示</t>
         </is>
       </c>
       <c r="D10" s="9" t="inlineStr"/>
@@ -1391,17 +1577,17 @@
     <row r="11">
       <c r="A11" s="10" t="inlineStr">
         <is>
-          <t>❌ 未完了</t>
+          <t>⚠️ 一部完了</t>
         </is>
       </c>
       <c r="B11" s="9" t="inlineStr">
         <is>
-          <t>投稿一覧表示</t>
+          <t>投稿機能</t>
         </is>
       </c>
       <c r="C11" s="9" t="inlineStr">
         <is>
-          <t>開発中</t>
+          <t>表示のみ完了、入力フォームは今後開発</t>
         </is>
       </c>
       <c r="D11" s="9" t="inlineStr"/>
@@ -1444,7 +1630,7 @@
     <row r="15">
       <c r="A15" s="12" t="inlineStr">
         <is>
-          <t>02/02 (Mon)</t>
+          <t>02/03 (Tue)</t>
         </is>
       </c>
       <c r="B15" s="12" t="inlineStr">
@@ -1454,7 +1640,7 @@
       </c>
       <c r="C15" s="12" t="inlineStr">
         <is>
-          <t>ヒデさん</t>
+          <t>本田</t>
         </is>
       </c>
       <c r="D15" s="12" t="inlineStr">
@@ -1471,17 +1657,17 @@
     <row r="16">
       <c r="A16" s="12" t="inlineStr">
         <is>
-          <t>02/02 (Mon)</t>
+          <t>02/03 (Tue)</t>
         </is>
       </c>
       <c r="B16" s="12" t="inlineStr">
         <is>
-          <t>社長からのフィードバック収集</t>
+          <t>三津谷社長からのフィードバック収集</t>
         </is>
       </c>
       <c r="C16" s="12" t="inlineStr">
         <is>
-          <t>ヒデさん</t>
+          <t>本田</t>
         </is>
       </c>
       <c r="D16" s="12" t="inlineStr">
@@ -1498,7 +1684,7 @@
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>02/03 (Tue)</t>
+          <t>02/04 (Wed)</t>
         </is>
       </c>
       <c r="B17" s="4" t="inlineStr">
@@ -1525,7 +1711,7 @@
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
         <is>
-          <t>02/04 (Wed)</t>
+          <t>02/05 (Thu)</t>
         </is>
       </c>
       <c r="B18" s="4" t="inlineStr">
@@ -1552,7 +1738,7 @@
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>02/05 (Thu)</t>
+          <t>02/06 (Fri)</t>
         </is>
       </c>
       <c r="B19" s="4" t="inlineStr">
@@ -1579,7 +1765,7 @@
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>02/06 (Fri)</t>
+          <t>02/07 (Sat)</t>
         </is>
       </c>
       <c r="B20" s="4" t="inlineStr">
@@ -1606,7 +1792,7 @@
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>02/06 (Fri)</t>
+          <t>02/07 (Sat)</t>
         </is>
       </c>
       <c r="B21" s="4" t="inlineStr">
@@ -1633,7 +1819,7 @@
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>02/07 (Sat)</t>
+          <t>02/08 (Sun)</t>
         </is>
       </c>
       <c r="B22" s="4" t="inlineStr">
@@ -1643,7 +1829,7 @@
       </c>
       <c r="C22" s="4" t="inlineStr">
         <is>
-          <t>ヒデさん</t>
+          <t>本田</t>
         </is>
       </c>
       <c r="D22" s="4" t="inlineStr">
@@ -1660,7 +1846,7 @@
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>02/08 (Sun)</t>
+          <t>02/09 (Mon)</t>
         </is>
       </c>
       <c r="B23" s="4" t="inlineStr">
@@ -1687,7 +1873,7 @@
     <row r="24">
       <c r="A24" s="4" t="inlineStr">
         <is>
-          <t>02/09 (Mon)</t>
+          <t>02/10 (Tue)</t>
         </is>
       </c>
       <c r="B24" s="4" t="inlineStr">
@@ -1697,7 +1883,7 @@
       </c>
       <c r="C24" s="4" t="inlineStr">
         <is>
-          <t>ヒデさん</t>
+          <t>本田</t>
         </is>
       </c>
       <c r="D24" s="4" t="inlineStr">

</xml_diff>